<commit_message>
Remove ELCD generation by power plants
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_BIO_10.xlsx
+++ b/SuppXLS/Scen_ELC_BIO_10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E172D97A-2788-463A-A041-2D57CE7E8735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C593D79-B8F8-4727-9D20-6C6B489BFAFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="4" r:id="rId1"/>
@@ -116,10 +116,6 @@
     <t>Pset_PD</t>
   </si>
   <si>
-    <t>ELCC,ELCD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>P*BIO*</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -340,6 +336,9 @@
   </si>
   <si>
     <t>Max BIO Penetration</t>
+  </si>
+  <si>
+    <t>ELCC</t>
   </si>
 </sst>
 </file>
@@ -1047,13 +1046,13 @@
     </row>
     <row r="5" spans="1:30" ht="15">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="E5" s="2" t="str">
         <f>A11</f>
@@ -1162,7 +1161,7 @@
     </row>
     <row r="6" spans="1:30" ht="15">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="str">
         <f>C5</f>
@@ -1279,7 +1278,7 @@
     </row>
     <row r="7" spans="1:30" ht="15">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="str">
         <f>"*"&amp;C5</f>
@@ -1396,223 +1395,223 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1">
       <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:30">
       <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15">
       <c r="A37" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1657,7 +1656,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G9:G15"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1697,7 +1696,7 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1762,7 +1761,7 @@
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I8" t="s">
         <v>5</v>
@@ -1771,7 +1770,7 @@
         <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L8" t="s">
         <v>9</v>
@@ -1785,16 +1784,16 @@
     </row>
     <row r="9" spans="1:14">
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="H9">
         <v>2020</v>
@@ -1816,12 +1815,12 @@
         <v>15</v>
       </c>
       <c r="N9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="G10" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="H10">
         <v>2025</v>
@@ -1833,7 +1832,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="G11" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="H11">
         <v>2030</v>
@@ -1845,7 +1844,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="G12" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="H12">
         <v>2035</v>
@@ -1857,7 +1856,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="G13" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="H13">
         <v>2040</v>
@@ -1869,7 +1868,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="G14" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="H14">
         <v>2045</v>
@@ -1881,7 +1880,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="G15" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="H15">
         <v>2050</v>

</xml_diff>